<commit_message>
1. Added rest end point to full trip 2. Added data on auxilary tabs by formula
</commit_message>
<xml_diff>
--- a/src/main/resources/template.xlsx
+++ b/src/main/resources/template.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/oleksii/kerriline/uz-location/src/main/resources/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{16154A0F-E0FF-4244-984C-400D2456DA1F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EB5291BB-12AF-9043-811A-09376F2C5135}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="500" windowWidth="28800" windowHeight="15800" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -17,22 +17,21 @@
     <sheet name="Полувагоны" sheetId="2" r:id="rId2"/>
     <sheet name="Вагоны" sheetId="3" r:id="rId3"/>
     <sheet name="Не полувагоны" sheetId="4" r:id="rId4"/>
-    <sheet name="Инструкция" sheetId="5" r:id="rId5"/>
-    <sheet name="Соответствие2" sheetId="7" state="hidden" r:id="rId6"/>
+    <sheet name="Соответствие2" sheetId="7" state="hidden" r:id="rId5"/>
   </sheets>
   <definedNames>
     <definedName name="_xlnm._FilterDatabase" localSheetId="2" hidden="1">Вагоны!$A$2:$D$2</definedName>
     <definedName name="_xlnm._FilterDatabase" localSheetId="3" hidden="1">'Не полувагоны'!$A$3:$AS$120</definedName>
     <definedName name="_xlnm._FilterDatabase" localSheetId="1" hidden="1">Полувагоны!$A$3:$AS$3</definedName>
     <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Результат!$A$3:$AI$3</definedName>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="5" hidden="1">Соответствие2!$A$1:$D$78</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="4" hidden="1">Соответствие2!$A$1:$D$78</definedName>
     <definedName name="Z_8DD274BA_7711_434E_BA5B_5A3C3CA953AD_.wvu.FilterData" localSheetId="0" hidden="1">Результат!$A$3:$AI$3</definedName>
     <definedName name="Z_EE108735_F011_40B2_BD14_38E8F8DDC1B4_.wvu.FilterData" localSheetId="2" hidden="1">Вагоны!$A$2:$D$2</definedName>
   </definedNames>
   <calcPr calcId="191029"/>
   <customWorkbookViews>
+    <customWorkbookView name="Сорт по ваг" guid="{EE108735-F011-40B2-BD14-38E8F8DDC1B4}" maximized="1" windowWidth="0" windowHeight="0" activeSheetId="0"/>
     <customWorkbookView name="Фільтр 1" guid="{8DD274BA-7711-434E-BA5B-5A3C3CA953AD}" maximized="1" windowWidth="0" windowHeight="0" activeSheetId="0"/>
-    <customWorkbookView name="Сорт по ваг" guid="{EE108735-F011-40B2-BD14-38E8F8DDC1B4}" maximized="1" windowWidth="0" windowHeight="0" activeSheetId="0"/>
   </customWorkbookViews>
   <extLst>
     <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
@@ -48,8 +47,30 @@
 </workbook>
 </file>
 
+<file path=xl/metadata.xml><?xml version="1.0" encoding="utf-8"?>
+<metadata xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:xda="http://schemas.microsoft.com/office/spreadsheetml/2017/dynamicarray">
+  <metadataTypes count="1">
+    <metadataType name="XLDAPR" minSupportedVersion="120000" copy="1" pasteAll="1" pasteValues="1" merge="1" splitFirst="1" rowColShift="1" clearFormats="1" clearComments="1" assign="1" coerce="1" cellMeta="1"/>
+  </metadataTypes>
+  <futureMetadata name="XLDAPR" count="1">
+    <bk>
+      <extLst>
+        <ext uri="{bdbb8cdc-fa1e-496e-a857-3c3f30c029c3}">
+          <xda:dynamicArrayProperties fDynamic="1" fCollapsed="0"/>
+        </ext>
+      </extLst>
+    </bk>
+  </futureMetadata>
+  <cellMetadata count="1">
+    <bk>
+      <rc t="1" v="0"/>
+    </bk>
+  </cellMetadata>
+</metadata>
+</file>
+
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="283" uniqueCount="178">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="275" uniqueCount="170">
   <si>
     <t>Дислокация</t>
   </si>
@@ -158,84 +179,6 @@
   </si>
   <si>
     <t>Неисправность</t>
-  </si>
-  <si>
-    <t>Проблем с производительностью в MS Excel</t>
-  </si>
-  <si>
-    <t>1. Заходим в файл Дислокация в Google Sheets по ссылке https://docs.google.com/spreadsheets/d/1nvt2kZB_VQV8Q8rHjfoYradT2sL_rzrkwEpTO6rWyTw/edit#gid=315911869</t>
-  </si>
-  <si>
-    <r>
-      <t xml:space="preserve">2. Переименновуем лист </t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="10"/>
-        <rFont val="Arial"/>
-      </rPr>
-      <t>Результат</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <color rgb="FF000000"/>
-        <rFont val="Arial"/>
-      </rPr>
-      <t xml:space="preserve"> в Рельзутат-Старый</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <t xml:space="preserve">3. Создаем новый лист с названием </t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="10"/>
-        <rFont val="Arial"/>
-      </rPr>
-      <t>Результат</t>
-    </r>
-  </si>
-  <si>
-    <t>4. Копируем со старого листа шапку</t>
-  </si>
-  <si>
-    <t>5. Формируем отчет - открываем следующую ссылку на сервере C:/uz-location/links/0 - Запросить справку - сформировать отчет и отправить на почту</t>
-  </si>
-  <si>
-    <r>
-      <t xml:space="preserve">6. Ставим фильтры - выделяем третюю строку, переходим в меню </t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="10"/>
-        <rFont val="Arial"/>
-      </rPr>
-      <t>Данные</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <color rgb="FF000000"/>
-        <rFont val="Arial"/>
-      </rPr>
-      <t xml:space="preserve"> - </t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="10"/>
-        <rFont val="Arial"/>
-      </rPr>
-      <t>Создать фильтр</t>
-    </r>
-  </si>
-  <si>
-    <t>7. Создаем правили условного форматирования на диапазон A4:D2046, формат ячеек Ваша формула - =IF(VALUE(SUBSTITUTE($AD$4:$AD$2046; "-";":")) &gt; VALUE(SUBSTITUTE($AH$4:$AH$2046; "-";":"));"Да";"Нет")="Да"</t>
   </si>
   <si>
     <t>Номер</t>
@@ -647,7 +590,7 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="yyyy\.mm\.dd\ hh:mm:ss"/>
   </numFmts>
-  <fonts count="7" x14ac:knownFonts="1">
+  <fonts count="6" x14ac:knownFonts="1">
     <font>
       <sz val="10"/>
       <color rgb="FF000000"/>
@@ -656,29 +599,29 @@
     <font>
       <sz val="10"/>
       <name val="Arial"/>
+      <family val="2"/>
     </font>
     <font>
       <sz val="10"/>
       <name val="Arial"/>
+      <family val="2"/>
     </font>
     <font>
       <b/>
       <sz val="11"/>
       <name val="Arial"/>
+      <family val="2"/>
     </font>
     <font>
       <sz val="11"/>
       <name val="Arial"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="10"/>
-      <name val="Arial"/>
+      <family val="2"/>
     </font>
     <font>
       <sz val="10"/>
       <color rgb="FF222222"/>
       <name val="Arial"/>
+      <family val="2"/>
     </font>
   </fonts>
   <fills count="5">
@@ -830,7 +773,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="39">
+  <cellXfs count="38">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
@@ -887,17 +830,16 @@
     <xf numFmtId="0" fontId="4" fillId="4" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="4" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyFont="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="6" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="6" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="5" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="5" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -910,7 +852,27 @@
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="2">
+  <dxfs count="4">
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
     <dxf>
       <fill>
         <patternFill patternType="solid">
@@ -1244,7 +1206,7 @@
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="3" topLeftCell="A4" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="C28" sqref="C28"/>
+      <selection pane="bottomLeft" activeCell="A4" sqref="A4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="14.5" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
@@ -1292,47 +1254,47 @@
       <c r="C1" s="2"/>
       <c r="D1" s="2"/>
       <c r="E1" s="2"/>
-      <c r="F1" s="38"/>
-      <c r="G1" s="36"/>
-      <c r="H1" s="36"/>
-      <c r="I1" s="36"/>
-      <c r="J1" s="35" t="s">
+      <c r="F1" s="37"/>
+      <c r="G1" s="35"/>
+      <c r="H1" s="35"/>
+      <c r="I1" s="35"/>
+      <c r="J1" s="34" t="s">
         <v>0</v>
       </c>
-      <c r="K1" s="36"/>
-      <c r="L1" s="36"/>
-      <c r="M1" s="36"/>
-      <c r="N1" s="37"/>
-      <c r="O1" s="35" t="s">
+      <c r="K1" s="35"/>
+      <c r="L1" s="35"/>
+      <c r="M1" s="35"/>
+      <c r="N1" s="36"/>
+      <c r="O1" s="34" t="s">
         <v>1</v>
       </c>
-      <c r="P1" s="36"/>
-      <c r="Q1" s="36"/>
-      <c r="R1" s="36"/>
-      <c r="S1" s="36"/>
-      <c r="T1" s="37"/>
+      <c r="P1" s="35"/>
+      <c r="Q1" s="35"/>
+      <c r="R1" s="35"/>
+      <c r="S1" s="35"/>
+      <c r="T1" s="36"/>
       <c r="U1" s="3" t="s">
         <v>2</v>
       </c>
-      <c r="V1" s="35" t="s">
+      <c r="V1" s="34" t="s">
         <v>3</v>
       </c>
-      <c r="W1" s="36"/>
-      <c r="X1" s="36"/>
-      <c r="Y1" s="37"/>
+      <c r="W1" s="35"/>
+      <c r="X1" s="35"/>
+      <c r="Y1" s="36"/>
       <c r="Z1" s="4"/>
       <c r="AA1" s="5"/>
-      <c r="AB1" s="35" t="s">
+      <c r="AB1" s="34" t="s">
         <v>4</v>
       </c>
-      <c r="AC1" s="36"/>
-      <c r="AD1" s="36"/>
-      <c r="AE1" s="37"/>
-      <c r="AF1" s="35" t="s">
+      <c r="AC1" s="35"/>
+      <c r="AD1" s="35"/>
+      <c r="AE1" s="36"/>
+      <c r="AF1" s="34" t="s">
         <v>5</v>
       </c>
-      <c r="AG1" s="36"/>
-      <c r="AH1" s="37"/>
+      <c r="AG1" s="35"/>
+      <c r="AH1" s="36"/>
       <c r="AI1" s="6"/>
     </row>
     <row r="2" spans="1:35" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
@@ -4416,7 +4378,7 @@
   <customSheetViews>
     <customSheetView guid="{8DD274BA-7711-434E-BA5B-5A3C3CA953AD}" filter="1" showAutoFilter="1">
       <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-      <autoFilter ref="A3:AI3" xr:uid="{1D599986-68D3-DE4C-BF10-328C95AE94FB}"/>
+      <autoFilter ref="A3:AI3" xr:uid="{FDBC90BB-6EFB-1E4F-9F0D-1F5FDE8F0550}"/>
     </customSheetView>
   </customSheetViews>
   <mergeCells count="6">
@@ -4427,6 +4389,11 @@
     <mergeCell ref="V1:Y1"/>
     <mergeCell ref="AB1:AE1"/>
   </mergeCells>
+  <conditionalFormatting sqref="B4:D5000">
+    <cfRule type="expression" dxfId="1" priority="1">
+      <formula>DATEVALUE(SUBSTITUTE($AD4:$AD5000,"-",":"))&gt;DATEVALUE(SUBSTITUTE($AH4:$AH5000,"-",":"))</formula>
+    </cfRule>
+  </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
@@ -4436,11 +4403,11 @@
   <sheetPr>
     <outlinePr summaryBelow="0" summaryRight="0"/>
   </sheetPr>
-  <dimension ref="A1:AI3"/>
+  <dimension ref="A1:AI4"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <pane ySplit="3" topLeftCell="A4" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="A4" sqref="A4:XFD444"/>
+      <selection pane="bottomLeft" activeCell="C16" sqref="C16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="14.5" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
@@ -4488,47 +4455,47 @@
       <c r="C1" s="2"/>
       <c r="D1" s="2"/>
       <c r="E1" s="2"/>
-      <c r="F1" s="38"/>
-      <c r="G1" s="36"/>
-      <c r="H1" s="36"/>
-      <c r="I1" s="36"/>
-      <c r="J1" s="35" t="s">
+      <c r="F1" s="37"/>
+      <c r="G1" s="35"/>
+      <c r="H1" s="35"/>
+      <c r="I1" s="35"/>
+      <c r="J1" s="34" t="s">
         <v>0</v>
       </c>
-      <c r="K1" s="36"/>
-      <c r="L1" s="36"/>
-      <c r="M1" s="36"/>
-      <c r="N1" s="37"/>
-      <c r="O1" s="35" t="s">
+      <c r="K1" s="35"/>
+      <c r="L1" s="35"/>
+      <c r="M1" s="35"/>
+      <c r="N1" s="36"/>
+      <c r="O1" s="34" t="s">
         <v>1</v>
       </c>
-      <c r="P1" s="36"/>
-      <c r="Q1" s="36"/>
-      <c r="R1" s="36"/>
-      <c r="S1" s="36"/>
-      <c r="T1" s="37"/>
+      <c r="P1" s="35"/>
+      <c r="Q1" s="35"/>
+      <c r="R1" s="35"/>
+      <c r="S1" s="35"/>
+      <c r="T1" s="36"/>
       <c r="U1" s="3" t="s">
         <v>2</v>
       </c>
-      <c r="V1" s="35" t="s">
+      <c r="V1" s="34" t="s">
         <v>3</v>
       </c>
-      <c r="W1" s="36"/>
-      <c r="X1" s="36"/>
-      <c r="Y1" s="37"/>
+      <c r="W1" s="35"/>
+      <c r="X1" s="35"/>
+      <c r="Y1" s="36"/>
       <c r="Z1" s="4"/>
       <c r="AA1" s="5"/>
-      <c r="AB1" s="35" t="s">
+      <c r="AB1" s="34" t="s">
         <v>4</v>
       </c>
-      <c r="AC1" s="36"/>
-      <c r="AD1" s="36"/>
-      <c r="AE1" s="37"/>
-      <c r="AF1" s="35" t="s">
+      <c r="AC1" s="35"/>
+      <c r="AD1" s="35"/>
+      <c r="AE1" s="36"/>
+      <c r="AF1" s="34" t="s">
         <v>5</v>
       </c>
-      <c r="AG1" s="36"/>
-      <c r="AH1" s="37"/>
+      <c r="AG1" s="35"/>
+      <c r="AH1" s="36"/>
       <c r="AI1" s="12"/>
     </row>
     <row r="2" spans="1:35" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
@@ -4743,6 +4710,12 @@
       </c>
       <c r="AI3" s="20">
         <v>35</v>
+      </c>
+    </row>
+    <row r="4" spans="1:35" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A4" t="str" cm="1">
+        <f t="array" ref="A4">_xlfn._xlws.FILTER(Результат!$A$4:$Y$5000,(Результат!$E$4:$E$5000="60 ПОЛУВАГОНЫ")+(Результат!$E$4:$E$5000="68 ГЛУХОДОННЫЕ"),"")</f>
+        <v/>
       </c>
     </row>
   </sheetData>
@@ -4760,7 +4733,7 @@
     <mergeCell ref="AB1:AE1"/>
   </mergeCells>
   <conditionalFormatting sqref="E4:E562">
-    <cfRule type="expression" dxfId="1" priority="1">
+    <cfRule type="expression" dxfId="3" priority="1">
       <formula>IF(VALUE(SUBSTITUTE($AD4:$AD1003, "-",":")) &gt; VALUE(SUBSTITUTE($AH4:$AH1003, "-",":")),"Да","Нет")="Да"</formula>
     </cfRule>
   </conditionalFormatting>
@@ -10655,7 +10628,7 @@
   <customSheetViews>
     <customSheetView guid="{EE108735-F011-40B2-BD14-38E8F8DDC1B4}" filter="1" showAutoFilter="1">
       <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-      <autoFilter ref="A2:D17" xr:uid="{EC715161-9172-C24E-8441-D40DD732CE31}">
+      <autoFilter ref="A2:D17" xr:uid="{260D271E-98ED-4240-BF85-6BB3CA28279A}">
         <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:D17">
           <sortCondition ref="D2:D17"/>
         </sortState>
@@ -10675,7 +10648,7 @@
   <sheetViews>
     <sheetView workbookViewId="0">
       <pane ySplit="3" topLeftCell="A4" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="A4" sqref="A4:XFD458"/>
+      <selection pane="bottomLeft" activeCell="A5" sqref="A5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="14.5" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
@@ -10723,47 +10696,47 @@
       <c r="C1" s="2"/>
       <c r="D1" s="2"/>
       <c r="E1" s="2"/>
-      <c r="F1" s="38"/>
-      <c r="G1" s="36"/>
-      <c r="H1" s="36"/>
-      <c r="I1" s="36"/>
-      <c r="J1" s="35" t="s">
+      <c r="F1" s="37"/>
+      <c r="G1" s="35"/>
+      <c r="H1" s="35"/>
+      <c r="I1" s="35"/>
+      <c r="J1" s="34" t="s">
         <v>0</v>
       </c>
-      <c r="K1" s="36"/>
-      <c r="L1" s="36"/>
-      <c r="M1" s="36"/>
-      <c r="N1" s="37"/>
-      <c r="O1" s="35" t="s">
+      <c r="K1" s="35"/>
+      <c r="L1" s="35"/>
+      <c r="M1" s="35"/>
+      <c r="N1" s="36"/>
+      <c r="O1" s="34" t="s">
         <v>1</v>
       </c>
-      <c r="P1" s="36"/>
-      <c r="Q1" s="36"/>
-      <c r="R1" s="36"/>
-      <c r="S1" s="36"/>
-      <c r="T1" s="37"/>
+      <c r="P1" s="35"/>
+      <c r="Q1" s="35"/>
+      <c r="R1" s="35"/>
+      <c r="S1" s="35"/>
+      <c r="T1" s="36"/>
       <c r="U1" s="3" t="s">
         <v>2</v>
       </c>
-      <c r="V1" s="35" t="s">
+      <c r="V1" s="34" t="s">
         <v>3</v>
       </c>
-      <c r="W1" s="36"/>
-      <c r="X1" s="36"/>
-      <c r="Y1" s="37"/>
+      <c r="W1" s="35"/>
+      <c r="X1" s="35"/>
+      <c r="Y1" s="36"/>
       <c r="Z1" s="4"/>
       <c r="AA1" s="5"/>
-      <c r="AB1" s="35" t="s">
+      <c r="AB1" s="34" t="s">
         <v>4</v>
       </c>
-      <c r="AC1" s="36"/>
-      <c r="AD1" s="36"/>
-      <c r="AE1" s="37"/>
-      <c r="AF1" s="35" t="s">
+      <c r="AC1" s="35"/>
+      <c r="AD1" s="35"/>
+      <c r="AE1" s="36"/>
+      <c r="AF1" s="34" t="s">
         <v>5</v>
       </c>
-      <c r="AG1" s="36"/>
-      <c r="AH1" s="37"/>
+      <c r="AG1" s="35"/>
+      <c r="AH1" s="36"/>
       <c r="AI1" s="12"/>
     </row>
     <row r="2" spans="1:35" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
@@ -10981,6 +10954,10 @@
       </c>
     </row>
     <row r="4" spans="1:35" ht="13" x14ac:dyDescent="0.15">
+      <c r="A4" t="str" cm="1">
+        <f t="array" ref="A4">_xlfn._xlws.FILTER(Результат!$A$4:$Y$5000,(Результат!$E$4:$E$5000&lt;&gt;"60 ПОЛУВАГОНЫ")*(Результат!$E$4:$E$5000&lt;&gt;"68 ГЛУХОДОННЫЕ")*(Результат!$E$4:$E$5000&lt;&gt;""),"")</f>
+        <v/>
+      </c>
       <c r="AI4" s="21"/>
     </row>
     <row r="5" spans="1:35" ht="13" x14ac:dyDescent="0.15">
@@ -13833,7 +13810,7 @@
     <mergeCell ref="AB1:AE1"/>
   </mergeCells>
   <conditionalFormatting sqref="E4:E1187">
-    <cfRule type="expression" dxfId="0" priority="1">
+    <cfRule type="expression" dxfId="2" priority="1">
       <formula>IF(VALUE(SUBSTITUTE($AD4:$AD1642, "-",":")) &gt; VALUE(SUBSTITUTE($AH4:$AH1642, "-",":")),"Да","Нет")="Да"</formula>
     </cfRule>
   </conditionalFormatting>
@@ -13842,65 +13819,6 @@
 </file>
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0400-000000000000}">
-  <sheetPr>
-    <outlinePr summaryBelow="0" summaryRight="0"/>
-  </sheetPr>
-  <dimension ref="A2:A9"/>
-  <sheetViews>
-    <sheetView workbookViewId="0"/>
-  </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="14.5" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
-  <cols>
-    <col min="1" max="1" width="105.33203125" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="2" spans="1:1" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A2" s="26" t="s">
-        <v>36</v>
-      </c>
-    </row>
-    <row r="3" spans="1:1" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A3" s="18" t="s">
-        <v>37</v>
-      </c>
-    </row>
-    <row r="4" spans="1:1" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A4" s="18" t="s">
-        <v>38</v>
-      </c>
-    </row>
-    <row r="5" spans="1:1" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A5" s="18" t="s">
-        <v>39</v>
-      </c>
-    </row>
-    <row r="6" spans="1:1" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A6" s="18" t="s">
-        <v>40</v>
-      </c>
-    </row>
-    <row r="7" spans="1:1" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A7" s="18" t="s">
-        <v>41</v>
-      </c>
-    </row>
-    <row r="8" spans="1:1" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A8" s="18" t="s">
-        <v>42</v>
-      </c>
-    </row>
-    <row r="9" spans="1:1" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A9" s="18" t="s">
-        <v>43</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0600-000000000000}">
   <sheetPr filterMode="1">
     <outlinePr summaryBelow="0" summaryRight="0"/>
@@ -13922,961 +13840,961 @@
   <sheetData>
     <row r="1" spans="1:4" ht="13" x14ac:dyDescent="0.15">
       <c r="A1" s="18" t="s">
+        <v>36</v>
+      </c>
+      <c r="B1" s="18" t="s">
+        <v>37</v>
+      </c>
+      <c r="C1" s="18" t="s">
+        <v>38</v>
+      </c>
+      <c r="D1" s="18" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4" ht="14" x14ac:dyDescent="0.15">
+      <c r="A2" s="27">
+        <v>4</v>
+      </c>
+      <c r="B2" s="28" t="s">
+        <v>40</v>
+      </c>
+      <c r="C2" s="18" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" ht="13" hidden="1" x14ac:dyDescent="0.15">
+      <c r="A3" s="26"/>
+      <c r="B3" s="28" t="s">
+        <v>42</v>
+      </c>
+      <c r="C3" s="18" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" ht="14" x14ac:dyDescent="0.15">
+      <c r="A4" s="27">
+        <v>24</v>
+      </c>
+      <c r="B4" s="28" t="s">
         <v>44</v>
       </c>
-      <c r="B1" s="18" t="s">
+      <c r="C4" s="18" t="s">
         <v>45</v>
       </c>
-      <c r="C1" s="18" t="s">
+    </row>
+    <row r="5" spans="1:4" ht="13" hidden="1" x14ac:dyDescent="0.15">
+      <c r="A5" s="26"/>
+      <c r="B5" s="28" t="s">
         <v>46</v>
       </c>
-      <c r="D1" s="18" t="s">
+      <c r="C5" s="18" t="s">
         <v>47</v>
       </c>
     </row>
-    <row r="2" spans="1:4" ht="14" x14ac:dyDescent="0.15">
-      <c r="A2" s="28">
-        <v>4</v>
-      </c>
-      <c r="B2" s="29" t="s">
+    <row r="6" spans="1:4" ht="13" hidden="1" x14ac:dyDescent="0.15">
+      <c r="A6" s="26"/>
+      <c r="B6" s="28" t="s">
         <v>48</v>
       </c>
-      <c r="C2" s="18" t="s">
+      <c r="C6" s="18" t="s">
         <v>49</v>
       </c>
     </row>
-    <row r="3" spans="1:4" ht="13" hidden="1" x14ac:dyDescent="0.15">
-      <c r="A3" s="27"/>
-      <c r="B3" s="29" t="s">
+    <row r="7" spans="1:4" ht="13" hidden="1" x14ac:dyDescent="0.15">
+      <c r="A7" s="26"/>
+      <c r="B7" s="28" t="s">
         <v>50</v>
       </c>
-      <c r="C3" s="18" t="s">
+      <c r="C7" s="18" t="s">
         <v>51</v>
       </c>
     </row>
-    <row r="4" spans="1:4" ht="14" x14ac:dyDescent="0.15">
-      <c r="A4" s="28">
-        <v>24</v>
-      </c>
-      <c r="B4" s="29" t="s">
+    <row r="8" spans="1:4" ht="13" hidden="1" x14ac:dyDescent="0.15">
+      <c r="A8" s="26"/>
+      <c r="B8" s="28" t="s">
         <v>52</v>
       </c>
-      <c r="C4" s="18" t="s">
+      <c r="C8" s="18" t="s">
         <v>53</v>
       </c>
     </row>
-    <row r="5" spans="1:4" ht="13" hidden="1" x14ac:dyDescent="0.15">
-      <c r="A5" s="27"/>
-      <c r="B5" s="29" t="s">
+    <row r="9" spans="1:4" ht="13" hidden="1" x14ac:dyDescent="0.15">
+      <c r="A9" s="26"/>
+      <c r="B9" s="28" t="s">
         <v>54</v>
       </c>
-      <c r="C5" s="18" t="s">
+      <c r="C9" s="18" t="s">
         <v>55</v>
       </c>
     </row>
-    <row r="6" spans="1:4" ht="13" hidden="1" x14ac:dyDescent="0.15">
-      <c r="A6" s="27"/>
-      <c r="B6" s="29" t="s">
+    <row r="10" spans="1:4" ht="14" x14ac:dyDescent="0.15">
+      <c r="A10" s="27">
+        <v>21</v>
+      </c>
+      <c r="B10" s="28" t="s">
         <v>56</v>
       </c>
-      <c r="C6" s="18" t="s">
+      <c r="C10" s="18" t="s">
         <v>57</v>
       </c>
     </row>
-    <row r="7" spans="1:4" ht="13" hidden="1" x14ac:dyDescent="0.15">
-      <c r="A7" s="27"/>
-      <c r="B7" s="29" t="s">
+    <row r="11" spans="1:4" ht="14" x14ac:dyDescent="0.15">
+      <c r="A11" s="27">
+        <v>5</v>
+      </c>
+      <c r="B11" s="28" t="s">
         <v>58</v>
       </c>
-      <c r="C7" s="18" t="s">
+      <c r="C11" s="18" t="s">
         <v>59</v>
       </c>
     </row>
-    <row r="8" spans="1:4" ht="13" hidden="1" x14ac:dyDescent="0.15">
-      <c r="A8" s="27"/>
-      <c r="B8" s="29" t="s">
+    <row r="12" spans="1:4" ht="13" hidden="1" x14ac:dyDescent="0.15">
+      <c r="A12" s="26"/>
+      <c r="B12" s="28" t="s">
         <v>60</v>
       </c>
-      <c r="C8" s="18" t="s">
+    </row>
+    <row r="13" spans="1:4" ht="13" hidden="1" x14ac:dyDescent="0.15">
+      <c r="A13" s="26"/>
+      <c r="B13" s="28" t="s">
         <v>61</v>
       </c>
     </row>
-    <row r="9" spans="1:4" ht="13" hidden="1" x14ac:dyDescent="0.15">
-      <c r="A9" s="27"/>
-      <c r="B9" s="29" t="s">
+    <row r="14" spans="1:4" ht="13" hidden="1" x14ac:dyDescent="0.15">
+      <c r="A14" s="26"/>
+      <c r="B14" s="28" t="s">
         <v>62</v>
       </c>
-      <c r="C9" s="18" t="s">
+    </row>
+    <row r="15" spans="1:4" ht="13" hidden="1" x14ac:dyDescent="0.15">
+      <c r="A15" s="26"/>
+      <c r="B15" s="28" t="s">
         <v>63</v>
       </c>
     </row>
-    <row r="10" spans="1:4" ht="14" x14ac:dyDescent="0.15">
-      <c r="A10" s="28">
-        <v>21</v>
-      </c>
-      <c r="B10" s="29" t="s">
+    <row r="16" spans="1:4" ht="14" x14ac:dyDescent="0.15">
+      <c r="A16" s="27">
+        <v>6.7</v>
+      </c>
+      <c r="B16" s="28" t="s">
         <v>64</v>
       </c>
-      <c r="C10" s="18" t="s">
+      <c r="C16" s="18" t="s">
         <v>65</v>
       </c>
     </row>
-    <row r="11" spans="1:4" ht="14" x14ac:dyDescent="0.15">
-      <c r="A11" s="28">
-        <v>5</v>
-      </c>
-      <c r="B11" s="29" t="s">
+    <row r="17" spans="1:3" ht="14" x14ac:dyDescent="0.15">
+      <c r="A17" s="27">
+        <v>15.16</v>
+      </c>
+      <c r="B17" s="28" t="s">
         <v>66</v>
       </c>
-      <c r="C11" s="18" t="s">
+      <c r="C17" s="18" t="s">
         <v>67</v>
       </c>
     </row>
-    <row r="12" spans="1:4" ht="13" hidden="1" x14ac:dyDescent="0.15">
-      <c r="A12" s="27"/>
-      <c r="B12" s="29" t="s">
+    <row r="18" spans="1:3" ht="14" x14ac:dyDescent="0.15">
+      <c r="A18" s="27">
+        <v>9</v>
+      </c>
+      <c r="B18" s="28" t="s">
         <v>68</v>
       </c>
-    </row>
-    <row r="13" spans="1:4" ht="13" hidden="1" x14ac:dyDescent="0.15">
-      <c r="A13" s="27"/>
-      <c r="B13" s="29" t="s">
+      <c r="C18" s="18" t="s">
         <v>69</v>
       </c>
     </row>
-    <row r="14" spans="1:4" ht="13" hidden="1" x14ac:dyDescent="0.15">
-      <c r="A14" s="27"/>
-      <c r="B14" s="29" t="s">
+    <row r="19" spans="1:3" ht="13" hidden="1" x14ac:dyDescent="0.15">
+      <c r="A19" s="26"/>
+      <c r="B19" s="28" t="s">
         <v>70</v>
       </c>
-    </row>
-    <row r="15" spans="1:4" ht="13" hidden="1" x14ac:dyDescent="0.15">
-      <c r="A15" s="27"/>
-      <c r="B15" s="29" t="s">
+      <c r="C19" s="18" t="s">
         <v>71</v>
       </c>
     </row>
-    <row r="16" spans="1:4" ht="14" x14ac:dyDescent="0.15">
-      <c r="A16" s="28">
-        <v>6.7</v>
-      </c>
-      <c r="B16" s="29" t="s">
+    <row r="20" spans="1:3" ht="14" x14ac:dyDescent="0.15">
+      <c r="A20" s="27">
+        <v>13</v>
+      </c>
+      <c r="B20" s="28" t="s">
         <v>72</v>
       </c>
-      <c r="C16" s="18" t="s">
+      <c r="C20" s="18" t="s">
         <v>73</v>
       </c>
     </row>
-    <row r="17" spans="1:3" ht="14" x14ac:dyDescent="0.15">
-      <c r="A17" s="28">
-        <v>15.16</v>
-      </c>
-      <c r="B17" s="29" t="s">
+    <row r="21" spans="1:3" ht="14" x14ac:dyDescent="0.15">
+      <c r="A21" s="27">
+        <v>11.12</v>
+      </c>
+      <c r="B21" s="28" t="s">
         <v>74</v>
       </c>
-      <c r="C17" s="18" t="s">
+      <c r="C21" s="18" t="s">
         <v>75</v>
       </c>
     </row>
-    <row r="18" spans="1:3" ht="14" x14ac:dyDescent="0.15">
-      <c r="A18" s="28">
-        <v>9</v>
-      </c>
-      <c r="B18" s="29" t="s">
+    <row r="22" spans="1:3" ht="14" x14ac:dyDescent="0.15">
+      <c r="A22" s="27">
+        <v>14</v>
+      </c>
+      <c r="B22" s="28" t="s">
         <v>76</v>
       </c>
-      <c r="C18" s="18" t="s">
+      <c r="C22" s="18" t="s">
         <v>77</v>
       </c>
     </row>
-    <row r="19" spans="1:3" ht="13" hidden="1" x14ac:dyDescent="0.15">
-      <c r="A19" s="27"/>
-      <c r="B19" s="29" t="s">
+    <row r="23" spans="1:3" ht="13" hidden="1" x14ac:dyDescent="0.15">
+      <c r="A23" s="26"/>
+      <c r="B23" s="28" t="s">
         <v>78</v>
       </c>
-      <c r="C19" s="18" t="s">
+      <c r="C23" s="18" t="s">
         <v>79</v>
       </c>
     </row>
-    <row r="20" spans="1:3" ht="14" x14ac:dyDescent="0.15">
-      <c r="A20" s="28">
-        <v>13</v>
-      </c>
-      <c r="B20" s="29" t="s">
+    <row r="24" spans="1:3" ht="14" x14ac:dyDescent="0.15">
+      <c r="A24" s="27">
+        <v>10</v>
+      </c>
+      <c r="B24" s="28" t="s">
         <v>80</v>
       </c>
-      <c r="C20" s="18" t="s">
+      <c r="C24" s="28" t="s">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="25" spans="1:3" ht="13" hidden="1" x14ac:dyDescent="0.15">
+      <c r="A25" s="26"/>
+      <c r="B25" s="29" t="s">
         <v>81</v>
       </c>
     </row>
-    <row r="21" spans="1:3" ht="14" x14ac:dyDescent="0.15">
-      <c r="A21" s="28">
-        <v>11.12</v>
-      </c>
-      <c r="B21" s="29" t="s">
+    <row r="26" spans="1:3" ht="13" hidden="1" x14ac:dyDescent="0.15">
+      <c r="A26" s="26"/>
+      <c r="B26" s="28" t="s">
         <v>82</v>
       </c>
-      <c r="C21" s="18" t="s">
+      <c r="C26" s="18" t="s">
         <v>83</v>
       </c>
     </row>
-    <row r="22" spans="1:3" ht="14" x14ac:dyDescent="0.15">
-      <c r="A22" s="28">
-        <v>14</v>
-      </c>
-      <c r="B22" s="29" t="s">
+    <row r="27" spans="1:3" ht="13" hidden="1" x14ac:dyDescent="0.15">
+      <c r="A27" s="26"/>
+      <c r="B27" s="28" t="s">
         <v>84</v>
       </c>
-      <c r="C22" s="18" t="s">
+      <c r="C27" s="18" t="s">
         <v>85</v>
       </c>
     </row>
-    <row r="23" spans="1:3" ht="13" hidden="1" x14ac:dyDescent="0.15">
-      <c r="A23" s="27"/>
-      <c r="B23" s="29" t="s">
+    <row r="28" spans="1:3" ht="13" hidden="1" x14ac:dyDescent="0.15">
+      <c r="A28" s="26"/>
+      <c r="B28" s="28" t="s">
         <v>86</v>
       </c>
-      <c r="C23" s="18" t="s">
+      <c r="C28" s="18" t="s">
         <v>87</v>
       </c>
     </row>
-    <row r="24" spans="1:3" ht="14" x14ac:dyDescent="0.15">
-      <c r="A24" s="28">
-        <v>10</v>
-      </c>
-      <c r="B24" s="29" t="s">
+    <row r="29" spans="1:3" ht="13" hidden="1" x14ac:dyDescent="0.15">
+      <c r="A29" s="26"/>
+      <c r="B29" s="28" t="s">
         <v>88</v>
       </c>
-      <c r="C24" s="29" t="s">
-        <v>88</v>
-      </c>
-    </row>
-    <row r="25" spans="1:3" ht="13" hidden="1" x14ac:dyDescent="0.15">
-      <c r="A25" s="27"/>
-      <c r="B25" s="30" t="s">
+      <c r="C29" s="18" t="s">
         <v>89</v>
       </c>
     </row>
-    <row r="26" spans="1:3" ht="13" hidden="1" x14ac:dyDescent="0.15">
-      <c r="A26" s="27"/>
-      <c r="B26" s="29" t="s">
+    <row r="30" spans="1:3" ht="13" hidden="1" x14ac:dyDescent="0.15">
+      <c r="A30" s="26"/>
+      <c r="B30" s="28" t="s">
         <v>90</v>
       </c>
-      <c r="C26" s="18" t="s">
+      <c r="C30" s="18" t="s">
         <v>91</v>
       </c>
     </row>
-    <row r="27" spans="1:3" ht="13" hidden="1" x14ac:dyDescent="0.15">
-      <c r="A27" s="27"/>
-      <c r="B27" s="29" t="s">
+    <row r="31" spans="1:3" ht="13" hidden="1" x14ac:dyDescent="0.15">
+      <c r="A31" s="26"/>
+      <c r="B31" s="28" t="s">
+        <v>66</v>
+      </c>
+      <c r="C31" s="18" t="s">
         <v>92</v>
       </c>
-      <c r="C27" s="18" t="s">
+    </row>
+    <row r="32" spans="1:3" ht="14" x14ac:dyDescent="0.15">
+      <c r="A32" s="27">
+        <v>20</v>
+      </c>
+      <c r="B32" s="28" t="s">
         <v>93</v>
       </c>
-    </row>
-    <row r="28" spans="1:3" ht="13" hidden="1" x14ac:dyDescent="0.15">
-      <c r="A28" s="27"/>
-      <c r="B28" s="29" t="s">
+      <c r="C32" s="18" t="s">
         <v>94</v>
       </c>
-      <c r="C28" s="18" t="s">
+    </row>
+    <row r="33" spans="1:3" ht="13" hidden="1" x14ac:dyDescent="0.15">
+      <c r="A33" s="26"/>
+      <c r="B33" s="28" t="s">
+        <v>68</v>
+      </c>
+      <c r="C33" s="18" t="s">
         <v>95</v>
       </c>
     </row>
-    <row r="29" spans="1:3" ht="13" hidden="1" x14ac:dyDescent="0.15">
-      <c r="A29" s="27"/>
-      <c r="B29" s="29" t="s">
+    <row r="34" spans="1:3" ht="13" hidden="1" x14ac:dyDescent="0.15">
+      <c r="A34" s="26"/>
+      <c r="B34" s="29" t="s">
         <v>96</v>
       </c>
-      <c r="C29" s="18" t="s">
+    </row>
+    <row r="35" spans="1:3" ht="13" hidden="1" x14ac:dyDescent="0.15">
+      <c r="A35" s="26"/>
+      <c r="B35" s="28" t="s">
         <v>97</v>
       </c>
-    </row>
-    <row r="30" spans="1:3" ht="13" hidden="1" x14ac:dyDescent="0.15">
-      <c r="A30" s="27"/>
-      <c r="B30" s="29" t="s">
+      <c r="C35" s="18" t="s">
         <v>98</v>
       </c>
-      <c r="C30" s="18" t="s">
+    </row>
+    <row r="36" spans="1:3" ht="13" hidden="1" x14ac:dyDescent="0.15">
+      <c r="A36" s="26"/>
+      <c r="B36" s="28" t="s">
         <v>99</v>
       </c>
-    </row>
-    <row r="31" spans="1:3" ht="13" hidden="1" x14ac:dyDescent="0.15">
-      <c r="A31" s="27"/>
-      <c r="B31" s="29" t="s">
-        <v>74</v>
-      </c>
-      <c r="C31" s="18" t="s">
+      <c r="C36" s="18" t="s">
         <v>100</v>
       </c>
     </row>
-    <row r="32" spans="1:3" ht="14" x14ac:dyDescent="0.15">
-      <c r="A32" s="28">
-        <v>20</v>
-      </c>
-      <c r="B32" s="29" t="s">
+    <row r="37" spans="1:3" ht="13" hidden="1" x14ac:dyDescent="0.15">
+      <c r="A37" s="26"/>
+      <c r="B37" s="28" t="s">
         <v>101</v>
       </c>
-      <c r="C32" s="18" t="s">
+      <c r="C37" s="18" t="s">
         <v>102</v>
       </c>
     </row>
-    <row r="33" spans="1:3" ht="13" hidden="1" x14ac:dyDescent="0.15">
-      <c r="A33" s="27"/>
-      <c r="B33" s="29" t="s">
-        <v>76</v>
-      </c>
-      <c r="C33" s="18" t="s">
+    <row r="38" spans="1:3" ht="14" x14ac:dyDescent="0.15">
+      <c r="A38" s="27">
+        <v>19</v>
+      </c>
+      <c r="B38" s="28" t="s">
         <v>103</v>
       </c>
-    </row>
-    <row r="34" spans="1:3" ht="13" hidden="1" x14ac:dyDescent="0.15">
-      <c r="A34" s="27"/>
-      <c r="B34" s="30" t="s">
+      <c r="C38" s="18" t="s">
         <v>104</v>
       </c>
     </row>
-    <row r="35" spans="1:3" ht="13" hidden="1" x14ac:dyDescent="0.15">
-      <c r="A35" s="27"/>
-      <c r="B35" s="29" t="s">
+    <row r="39" spans="1:3" ht="13" hidden="1" x14ac:dyDescent="0.15">
+      <c r="A39" s="26"/>
+      <c r="B39" s="28" t="s">
         <v>105</v>
       </c>
-      <c r="C35" s="18" t="s">
+      <c r="C39" s="18" t="s">
         <v>106</v>
       </c>
     </row>
-    <row r="36" spans="1:3" ht="13" hidden="1" x14ac:dyDescent="0.15">
-      <c r="A36" s="27"/>
-      <c r="B36" s="29" t="s">
+    <row r="40" spans="1:3" ht="13" hidden="1" x14ac:dyDescent="0.15">
+      <c r="A40" s="26"/>
+      <c r="B40" s="28" t="s">
         <v>107</v>
       </c>
-      <c r="C36" s="18" t="s">
+      <c r="C40" s="18" t="s">
         <v>108</v>
       </c>
     </row>
-    <row r="37" spans="1:3" ht="13" hidden="1" x14ac:dyDescent="0.15">
-      <c r="A37" s="27"/>
-      <c r="B37" s="29" t="s">
+    <row r="41" spans="1:3" ht="14" x14ac:dyDescent="0.15">
+      <c r="A41" s="27">
+        <v>17.18</v>
+      </c>
+      <c r="B41" s="28" t="s">
         <v>109</v>
       </c>
-      <c r="C37" s="18" t="s">
+      <c r="C41" s="18" t="s">
         <v>110</v>
       </c>
     </row>
-    <row r="38" spans="1:3" ht="14" x14ac:dyDescent="0.15">
-      <c r="A38" s="28">
-        <v>19</v>
-      </c>
-      <c r="B38" s="29" t="s">
+    <row r="42" spans="1:3" ht="14" x14ac:dyDescent="0.15">
+      <c r="A42" s="27">
+        <v>8</v>
+      </c>
+      <c r="B42" s="28" t="s">
         <v>111</v>
       </c>
-      <c r="C38" s="18" t="s">
+      <c r="C42" s="18" t="s">
         <v>112</v>
       </c>
     </row>
-    <row r="39" spans="1:3" ht="13" hidden="1" x14ac:dyDescent="0.15">
-      <c r="A39" s="27"/>
-      <c r="B39" s="29" t="s">
+    <row r="43" spans="1:3" ht="13" hidden="1" x14ac:dyDescent="0.15">
+      <c r="A43" s="26"/>
+      <c r="B43" s="28" t="s">
+        <v>90</v>
+      </c>
+      <c r="C43" s="18" t="s">
         <v>113</v>
       </c>
-      <c r="C39" s="18" t="s">
+    </row>
+    <row r="44" spans="1:3" ht="13" hidden="1" x14ac:dyDescent="0.15">
+      <c r="A44" s="26"/>
+      <c r="B44" s="28" t="s">
+        <v>93</v>
+      </c>
+      <c r="C44" s="18" t="s">
         <v>114</v>
       </c>
     </row>
-    <row r="40" spans="1:3" ht="13" hidden="1" x14ac:dyDescent="0.15">
-      <c r="A40" s="27"/>
-      <c r="B40" s="29" t="s">
+    <row r="45" spans="1:3" ht="13" hidden="1" x14ac:dyDescent="0.15">
+      <c r="A45" s="26"/>
+      <c r="B45" s="28" t="s">
+        <v>68</v>
+      </c>
+      <c r="C45" s="18" t="s">
         <v>115</v>
       </c>
-      <c r="C40" s="18" t="s">
+    </row>
+    <row r="46" spans="1:3" ht="13" hidden="1" x14ac:dyDescent="0.15">
+      <c r="A46" s="26"/>
+      <c r="B46" s="28" t="s">
+        <v>66</v>
+      </c>
+      <c r="C46" s="18" t="s">
         <v>116</v>
       </c>
     </row>
-    <row r="41" spans="1:3" ht="14" x14ac:dyDescent="0.15">
-      <c r="A41" s="28">
-        <v>17.18</v>
-      </c>
-      <c r="B41" s="29" t="s">
+    <row r="47" spans="1:3" ht="13" hidden="1" x14ac:dyDescent="0.15">
+      <c r="A47" s="26"/>
+      <c r="B47" s="28" t="s">
         <v>117</v>
       </c>
-      <c r="C41" s="18" t="s">
+      <c r="C47" s="18" t="s">
         <v>118</v>
       </c>
     </row>
-    <row r="42" spans="1:3" ht="14" x14ac:dyDescent="0.15">
-      <c r="A42" s="28">
-        <v>8</v>
-      </c>
-      <c r="B42" s="29" t="s">
+    <row r="48" spans="1:3" ht="13" hidden="1" x14ac:dyDescent="0.15">
+      <c r="A48" s="26"/>
+      <c r="B48" s="28" t="s">
         <v>119</v>
       </c>
-      <c r="C42" s="18" t="s">
+      <c r="C48" s="18" t="s">
         <v>120</v>
       </c>
     </row>
-    <row r="43" spans="1:3" ht="13" hidden="1" x14ac:dyDescent="0.15">
-      <c r="A43" s="27"/>
-      <c r="B43" s="29" t="s">
-        <v>98</v>
-      </c>
-      <c r="C43" s="18" t="s">
+    <row r="49" spans="1:3" ht="13" hidden="1" x14ac:dyDescent="0.15">
+      <c r="A49" s="26"/>
+      <c r="B49" s="28" t="s">
         <v>121</v>
       </c>
-    </row>
-    <row r="44" spans="1:3" ht="13" hidden="1" x14ac:dyDescent="0.15">
-      <c r="A44" s="27"/>
-      <c r="B44" s="29" t="s">
-        <v>101</v>
-      </c>
-      <c r="C44" s="18" t="s">
+      <c r="C49" s="18" t="s">
         <v>122</v>
       </c>
     </row>
-    <row r="45" spans="1:3" ht="13" hidden="1" x14ac:dyDescent="0.15">
-      <c r="A45" s="27"/>
-      <c r="B45" s="29" t="s">
-        <v>76</v>
-      </c>
-      <c r="C45" s="18" t="s">
+    <row r="50" spans="1:3" ht="13" hidden="1" x14ac:dyDescent="0.15">
+      <c r="A50" s="26"/>
+      <c r="B50" s="28" t="s">
         <v>123</v>
       </c>
-    </row>
-    <row r="46" spans="1:3" ht="13" hidden="1" x14ac:dyDescent="0.15">
-      <c r="A46" s="27"/>
-      <c r="B46" s="29" t="s">
-        <v>74</v>
-      </c>
-      <c r="C46" s="18" t="s">
+      <c r="C50" s="18" t="s">
         <v>124</v>
       </c>
     </row>
-    <row r="47" spans="1:3" ht="13" hidden="1" x14ac:dyDescent="0.15">
-      <c r="A47" s="27"/>
-      <c r="B47" s="29" t="s">
+    <row r="51" spans="1:3" ht="13" hidden="1" x14ac:dyDescent="0.15">
+      <c r="A51" s="26"/>
+      <c r="B51" s="28" t="s">
+        <v>105</v>
+      </c>
+      <c r="C51" s="18" t="s">
         <v>125</v>
       </c>
-      <c r="C47" s="18" t="s">
+    </row>
+    <row r="52" spans="1:3" ht="13" hidden="1" x14ac:dyDescent="0.15">
+      <c r="A52" s="26"/>
+      <c r="B52" s="28" t="s">
         <v>126</v>
       </c>
-    </row>
-    <row r="48" spans="1:3" ht="13" hidden="1" x14ac:dyDescent="0.15">
-      <c r="A48" s="27"/>
-      <c r="B48" s="29" t="s">
+      <c r="C52" s="18" t="s">
         <v>127</v>
       </c>
-      <c r="C48" s="18" t="s">
+    </row>
+    <row r="53" spans="1:3" ht="13" hidden="1" x14ac:dyDescent="0.15">
+      <c r="A53" s="26"/>
+      <c r="B53" s="28" t="s">
+        <v>107</v>
+      </c>
+      <c r="C53" s="18" t="s">
         <v>128</v>
       </c>
     </row>
-    <row r="49" spans="1:3" ht="13" hidden="1" x14ac:dyDescent="0.15">
-      <c r="A49" s="27"/>
-      <c r="B49" s="29" t="s">
+    <row r="54" spans="1:3" ht="13" hidden="1" x14ac:dyDescent="0.15">
+      <c r="A54" s="26"/>
+      <c r="B54" s="28" t="s">
         <v>129</v>
       </c>
-      <c r="C49" s="18" t="s">
+      <c r="C54" s="18" t="s">
         <v>130</v>
       </c>
     </row>
-    <row r="50" spans="1:3" ht="13" hidden="1" x14ac:dyDescent="0.15">
-      <c r="A50" s="27"/>
-      <c r="B50" s="29" t="s">
+    <row r="55" spans="1:3" ht="13" hidden="1" x14ac:dyDescent="0.15">
+      <c r="A55" s="26"/>
+      <c r="B55" s="28" t="s">
         <v>131</v>
       </c>
-      <c r="C50" s="18" t="s">
+      <c r="C55" s="18" t="s">
         <v>132</v>
       </c>
     </row>
-    <row r="51" spans="1:3" ht="13" hidden="1" x14ac:dyDescent="0.15">
-      <c r="A51" s="27"/>
-      <c r="B51" s="29" t="s">
-        <v>113</v>
-      </c>
-      <c r="C51" s="18" t="s">
+    <row r="56" spans="1:3" ht="13" hidden="1" x14ac:dyDescent="0.15">
+      <c r="A56" s="26"/>
+      <c r="B56" s="28" t="s">
         <v>133</v>
       </c>
-    </row>
-    <row r="52" spans="1:3" ht="13" hidden="1" x14ac:dyDescent="0.15">
-      <c r="A52" s="27"/>
-      <c r="B52" s="29" t="s">
+      <c r="C56" s="18" t="s">
         <v>134</v>
       </c>
-      <c r="C52" s="18" t="s">
+    </row>
+    <row r="57" spans="1:3" ht="13" hidden="1" x14ac:dyDescent="0.15">
+      <c r="A57" s="26"/>
+      <c r="B57" s="28" t="s">
         <v>135</v>
       </c>
-    </row>
-    <row r="53" spans="1:3" ht="13" hidden="1" x14ac:dyDescent="0.15">
-      <c r="A53" s="27"/>
-      <c r="B53" s="29" t="s">
-        <v>115</v>
-      </c>
-      <c r="C53" s="18" t="s">
+      <c r="C57" s="18" t="s">
         <v>136</v>
       </c>
     </row>
-    <row r="54" spans="1:3" ht="13" hidden="1" x14ac:dyDescent="0.15">
-      <c r="A54" s="27"/>
-      <c r="B54" s="29" t="s">
+    <row r="58" spans="1:3" ht="13" hidden="1" x14ac:dyDescent="0.15">
+      <c r="A58" s="26"/>
+      <c r="B58" s="28" t="s">
         <v>137</v>
       </c>
-      <c r="C54" s="18" t="s">
+    </row>
+    <row r="59" spans="1:3" ht="13" hidden="1" x14ac:dyDescent="0.15">
+      <c r="A59" s="26"/>
+      <c r="B59" s="28" t="s">
+        <v>90</v>
+      </c>
+      <c r="C59" s="18" t="s">
         <v>138</v>
       </c>
     </row>
-    <row r="55" spans="1:3" ht="13" hidden="1" x14ac:dyDescent="0.15">
-      <c r="A55" s="27"/>
-      <c r="B55" s="29" t="s">
+    <row r="60" spans="1:3" ht="13" hidden="1" x14ac:dyDescent="0.15">
+      <c r="A60" s="26"/>
+      <c r="B60" s="28" t="s">
         <v>139</v>
       </c>
-      <c r="C55" s="18" t="s">
+      <c r="C60" s="18" t="s">
         <v>140</v>
       </c>
     </row>
-    <row r="56" spans="1:3" ht="13" hidden="1" x14ac:dyDescent="0.15">
-      <c r="A56" s="27"/>
-      <c r="B56" s="29" t="s">
+    <row r="61" spans="1:3" ht="13" hidden="1" x14ac:dyDescent="0.15">
+      <c r="A61" s="26"/>
+      <c r="B61" s="28" t="s">
         <v>141</v>
       </c>
-      <c r="C56" s="18" t="s">
+      <c r="C61" s="18" t="s">
         <v>142</v>
       </c>
     </row>
-    <row r="57" spans="1:3" ht="13" hidden="1" x14ac:dyDescent="0.15">
-      <c r="A57" s="27"/>
-      <c r="B57" s="29" t="s">
+    <row r="62" spans="1:3" ht="13" hidden="1" x14ac:dyDescent="0.15">
+      <c r="A62" s="26"/>
+      <c r="B62" s="29" t="s">
         <v>143</v>
       </c>
-      <c r="C57" s="18" t="s">
+    </row>
+    <row r="63" spans="1:3" ht="14" x14ac:dyDescent="0.15">
+      <c r="A63" s="27">
+        <v>28</v>
+      </c>
+      <c r="B63" s="28" t="s">
         <v>144</v>
       </c>
-    </row>
-    <row r="58" spans="1:3" ht="13" hidden="1" x14ac:dyDescent="0.15">
-      <c r="A58" s="27"/>
-      <c r="B58" s="29" t="s">
+      <c r="C63" s="18" t="s">
         <v>145</v>
       </c>
     </row>
-    <row r="59" spans="1:3" ht="13" hidden="1" x14ac:dyDescent="0.15">
-      <c r="A59" s="27"/>
-      <c r="B59" s="29" t="s">
-        <v>98</v>
-      </c>
-      <c r="C59" s="18" t="s">
+    <row r="64" spans="1:3" ht="13" hidden="1" x14ac:dyDescent="0.15">
+      <c r="A64" s="26"/>
+      <c r="B64" s="28" t="s">
         <v>146</v>
       </c>
-    </row>
-    <row r="60" spans="1:3" ht="13" hidden="1" x14ac:dyDescent="0.15">
-      <c r="A60" s="27"/>
-      <c r="B60" s="29" t="s">
+      <c r="C64" s="18" t="s">
         <v>147</v>
       </c>
-      <c r="C60" s="18" t="s">
+    </row>
+    <row r="65" spans="1:3" ht="14" x14ac:dyDescent="0.15">
+      <c r="A65" s="27">
+        <v>26</v>
+      </c>
+      <c r="B65" s="28" t="s">
         <v>148</v>
       </c>
-    </row>
-    <row r="61" spans="1:3" ht="13" hidden="1" x14ac:dyDescent="0.15">
-      <c r="A61" s="27"/>
-      <c r="B61" s="29" t="s">
+      <c r="C65" s="18" t="s">
         <v>149</v>
       </c>
-      <c r="C61" s="18" t="s">
+    </row>
+    <row r="66" spans="1:3" ht="14" x14ac:dyDescent="0.15">
+      <c r="A66" s="27">
+        <v>27</v>
+      </c>
+      <c r="B66" s="28" t="s">
         <v>150</v>
       </c>
-    </row>
-    <row r="62" spans="1:3" ht="13" hidden="1" x14ac:dyDescent="0.15">
-      <c r="A62" s="27"/>
-      <c r="B62" s="30" t="s">
+      <c r="C66" s="18" t="s">
         <v>151</v>
       </c>
     </row>
-    <row r="63" spans="1:3" ht="14" x14ac:dyDescent="0.15">
-      <c r="A63" s="28">
-        <v>28</v>
-      </c>
-      <c r="B63" s="29" t="s">
+    <row r="67" spans="1:3" ht="13" hidden="1" x14ac:dyDescent="0.15">
+      <c r="A67" s="26"/>
+      <c r="B67" s="28" t="s">
         <v>152</v>
       </c>
-      <c r="C63" s="18" t="s">
+      <c r="C67" s="18" t="s">
         <v>153</v>
       </c>
     </row>
-    <row r="64" spans="1:3" ht="13" hidden="1" x14ac:dyDescent="0.15">
-      <c r="A64" s="27"/>
-      <c r="B64" s="29" t="s">
+    <row r="68" spans="1:3" ht="13" hidden="1" x14ac:dyDescent="0.15">
+      <c r="A68" s="26"/>
+      <c r="B68" s="28" t="s">
         <v>154</v>
       </c>
-      <c r="C64" s="18" t="s">
+      <c r="C68" s="18" t="s">
         <v>155</v>
       </c>
     </row>
-    <row r="65" spans="1:3" ht="14" x14ac:dyDescent="0.15">
-      <c r="A65" s="28">
-        <v>26</v>
-      </c>
-      <c r="B65" s="29" t="s">
+    <row r="69" spans="1:3" ht="14" x14ac:dyDescent="0.15">
+      <c r="A69" s="27">
+        <v>29</v>
+      </c>
+      <c r="B69" s="28" t="s">
         <v>156</v>
       </c>
-      <c r="C65" s="18" t="s">
+      <c r="C69" s="18" t="s">
         <v>157</v>
       </c>
     </row>
-    <row r="66" spans="1:3" ht="14" x14ac:dyDescent="0.15">
-      <c r="A66" s="28">
-        <v>27</v>
-      </c>
-      <c r="B66" s="29" t="s">
+    <row r="70" spans="1:3" ht="14" x14ac:dyDescent="0.15">
+      <c r="A70" s="27">
+        <v>32</v>
+      </c>
+      <c r="B70" s="28" t="s">
         <v>158</v>
       </c>
-      <c r="C66" s="18" t="s">
+      <c r="C70" s="18" t="s">
         <v>159</v>
       </c>
     </row>
-    <row r="67" spans="1:3" ht="13" hidden="1" x14ac:dyDescent="0.15">
-      <c r="A67" s="27"/>
-      <c r="B67" s="29" t="s">
+    <row r="71" spans="1:3" ht="13" hidden="1" x14ac:dyDescent="0.15">
+      <c r="A71" s="26"/>
+      <c r="B71" s="28" t="s">
+        <v>146</v>
+      </c>
+      <c r="C71" s="18" t="s">
         <v>160</v>
       </c>
-      <c r="C67" s="18" t="s">
+    </row>
+    <row r="72" spans="1:3" ht="14" x14ac:dyDescent="0.15">
+      <c r="A72" s="27">
+        <v>30</v>
+      </c>
+      <c r="B72" s="28" t="s">
+        <v>148</v>
+      </c>
+      <c r="C72" s="18" t="s">
         <v>161</v>
       </c>
     </row>
-    <row r="68" spans="1:3" ht="13" hidden="1" x14ac:dyDescent="0.15">
-      <c r="A68" s="27"/>
-      <c r="B68" s="29" t="s">
+    <row r="73" spans="1:3" ht="14" x14ac:dyDescent="0.15">
+      <c r="A73" s="27">
+        <v>31</v>
+      </c>
+      <c r="B73" s="28" t="s">
+        <v>150</v>
+      </c>
+      <c r="C73" s="18" t="s">
         <v>162</v>
       </c>
-      <c r="C68" s="18" t="s">
+    </row>
+    <row r="74" spans="1:3" ht="13" hidden="1" x14ac:dyDescent="0.15">
+      <c r="A74" s="26"/>
+      <c r="B74" s="30" t="s">
+        <v>152</v>
+      </c>
+      <c r="C74" s="18" t="s">
         <v>163</v>
       </c>
     </row>
-    <row r="69" spans="1:3" ht="14" x14ac:dyDescent="0.15">
-      <c r="A69" s="28">
-        <v>29</v>
-      </c>
-      <c r="B69" s="29" t="s">
+    <row r="75" spans="1:3" ht="13" hidden="1" x14ac:dyDescent="0.15">
+      <c r="A75" s="26"/>
+      <c r="B75" s="31"/>
+    </row>
+    <row r="76" spans="1:3" ht="14" x14ac:dyDescent="0.15">
+      <c r="A76" s="27">
+        <v>25</v>
+      </c>
+      <c r="B76" s="28" t="s">
         <v>164</v>
       </c>
-      <c r="C69" s="18" t="s">
+      <c r="C76" s="18" t="s">
         <v>165</v>
       </c>
     </row>
-    <row r="70" spans="1:3" ht="14" x14ac:dyDescent="0.15">
-      <c r="A70" s="28">
-        <v>32</v>
-      </c>
-      <c r="B70" s="29" t="s">
+    <row r="77" spans="1:3" ht="13" hidden="1" x14ac:dyDescent="0.15">
+      <c r="A77" s="26"/>
+      <c r="B77" s="28" t="s">
         <v>166</v>
       </c>
-      <c r="C70" s="18" t="s">
+      <c r="C77" s="18" t="s">
         <v>167</v>
       </c>
     </row>
-    <row r="71" spans="1:3" ht="13" hidden="1" x14ac:dyDescent="0.15">
-      <c r="A71" s="27"/>
-      <c r="B71" s="29" t="s">
-        <v>154</v>
-      </c>
-      <c r="C71" s="18" t="s">
+    <row r="78" spans="1:3" ht="13" hidden="1" x14ac:dyDescent="0.15">
+      <c r="A78" s="26"/>
+      <c r="B78" s="30" t="s">
         <v>168</v>
       </c>
-    </row>
-    <row r="72" spans="1:3" ht="14" x14ac:dyDescent="0.15">
-      <c r="A72" s="28">
-        <v>30</v>
-      </c>
-      <c r="B72" s="29" t="s">
-        <v>156</v>
-      </c>
-      <c r="C72" s="18" t="s">
+      <c r="C78" s="18" t="s">
         <v>169</v>
       </c>
     </row>
-    <row r="73" spans="1:3" ht="14" x14ac:dyDescent="0.15">
-      <c r="A73" s="28">
-        <v>31</v>
-      </c>
-      <c r="B73" s="29" t="s">
-        <v>158</v>
-      </c>
-      <c r="C73" s="18" t="s">
-        <v>170</v>
-      </c>
-    </row>
-    <row r="74" spans="1:3" ht="13" hidden="1" x14ac:dyDescent="0.15">
-      <c r="A74" s="27"/>
-      <c r="B74" s="31" t="s">
-        <v>160</v>
-      </c>
-      <c r="C74" s="18" t="s">
-        <v>171</v>
-      </c>
-    </row>
-    <row r="75" spans="1:3" ht="13" hidden="1" x14ac:dyDescent="0.15">
-      <c r="A75" s="27"/>
-      <c r="B75" s="32"/>
-    </row>
-    <row r="76" spans="1:3" ht="14" x14ac:dyDescent="0.15">
-      <c r="A76" s="28">
-        <v>25</v>
-      </c>
-      <c r="B76" s="29" t="s">
-        <v>172</v>
-      </c>
-      <c r="C76" s="18" t="s">
-        <v>173</v>
-      </c>
-    </row>
-    <row r="77" spans="1:3" ht="13" hidden="1" x14ac:dyDescent="0.15">
-      <c r="A77" s="27"/>
-      <c r="B77" s="29" t="s">
-        <v>174</v>
-      </c>
-      <c r="C77" s="18" t="s">
-        <v>175</v>
-      </c>
-    </row>
-    <row r="78" spans="1:3" ht="13" hidden="1" x14ac:dyDescent="0.15">
-      <c r="A78" s="27"/>
-      <c r="B78" s="31" t="s">
-        <v>176</v>
-      </c>
-      <c r="C78" s="18" t="s">
-        <v>177</v>
-      </c>
-    </row>
     <row r="79" spans="1:3" ht="13" x14ac:dyDescent="0.15">
-      <c r="B79" s="33"/>
+      <c r="B79" s="32"/>
     </row>
     <row r="80" spans="1:3" ht="13" x14ac:dyDescent="0.15">
-      <c r="B80" s="33"/>
+      <c r="B80" s="32"/>
     </row>
     <row r="81" spans="2:2" ht="13" x14ac:dyDescent="0.15">
-      <c r="B81" s="33"/>
+      <c r="B81" s="32"/>
     </row>
     <row r="82" spans="2:2" ht="13" x14ac:dyDescent="0.15">
-      <c r="B82" s="33"/>
+      <c r="B82" s="32"/>
     </row>
     <row r="83" spans="2:2" ht="13" x14ac:dyDescent="0.15">
-      <c r="B83" s="33"/>
+      <c r="B83" s="32"/>
     </row>
     <row r="84" spans="2:2" ht="13" x14ac:dyDescent="0.15">
-      <c r="B84" s="33"/>
+      <c r="B84" s="32"/>
     </row>
     <row r="85" spans="2:2" ht="13" x14ac:dyDescent="0.15">
-      <c r="B85" s="33"/>
+      <c r="B85" s="32"/>
     </row>
     <row r="86" spans="2:2" ht="13" x14ac:dyDescent="0.15">
-      <c r="B86" s="33"/>
+      <c r="B86" s="32"/>
     </row>
     <row r="87" spans="2:2" ht="13" x14ac:dyDescent="0.15">
-      <c r="B87" s="33"/>
+      <c r="B87" s="32"/>
     </row>
     <row r="88" spans="2:2" ht="13" x14ac:dyDescent="0.15">
-      <c r="B88" s="33"/>
+      <c r="B88" s="32"/>
     </row>
     <row r="89" spans="2:2" ht="13" x14ac:dyDescent="0.15">
-      <c r="B89" s="33"/>
+      <c r="B89" s="32"/>
     </row>
     <row r="90" spans="2:2" ht="13" x14ac:dyDescent="0.15">
-      <c r="B90" s="33"/>
+      <c r="B90" s="32"/>
     </row>
     <row r="91" spans="2:2" ht="13" x14ac:dyDescent="0.15">
-      <c r="B91" s="33"/>
+      <c r="B91" s="32"/>
     </row>
     <row r="92" spans="2:2" ht="13" x14ac:dyDescent="0.15">
-      <c r="B92" s="33"/>
+      <c r="B92" s="32"/>
     </row>
     <row r="93" spans="2:2" ht="13" x14ac:dyDescent="0.15">
-      <c r="B93" s="34"/>
+      <c r="B93" s="33"/>
     </row>
     <row r="94" spans="2:2" ht="13" x14ac:dyDescent="0.15">
-      <c r="B94" s="33"/>
+      <c r="B94" s="32"/>
     </row>
     <row r="95" spans="2:2" ht="13" x14ac:dyDescent="0.15">
-      <c r="B95" s="33"/>
+      <c r="B95" s="32"/>
     </row>
     <row r="96" spans="2:2" ht="13" x14ac:dyDescent="0.15">
-      <c r="B96" s="33"/>
+      <c r="B96" s="32"/>
     </row>
     <row r="97" spans="2:2" ht="13" x14ac:dyDescent="0.15">
-      <c r="B97" s="33"/>
+      <c r="B97" s="32"/>
     </row>
     <row r="98" spans="2:2" ht="13" x14ac:dyDescent="0.15">
-      <c r="B98" s="33"/>
+      <c r="B98" s="32"/>
     </row>
     <row r="99" spans="2:2" ht="13" x14ac:dyDescent="0.15">
-      <c r="B99" s="33"/>
+      <c r="B99" s="32"/>
     </row>
     <row r="100" spans="2:2" ht="13" x14ac:dyDescent="0.15">
-      <c r="B100" s="33"/>
+      <c r="B100" s="32"/>
     </row>
     <row r="101" spans="2:2" ht="13" x14ac:dyDescent="0.15">
-      <c r="B101" s="33"/>
+      <c r="B101" s="32"/>
     </row>
     <row r="102" spans="2:2" ht="13" x14ac:dyDescent="0.15">
-      <c r="B102" s="33"/>
+      <c r="B102" s="32"/>
     </row>
     <row r="103" spans="2:2" ht="13" x14ac:dyDescent="0.15">
-      <c r="B103" s="34"/>
+      <c r="B103" s="33"/>
     </row>
     <row r="104" spans="2:2" ht="13" x14ac:dyDescent="0.15">
-      <c r="B104" s="33"/>
+      <c r="B104" s="32"/>
     </row>
     <row r="105" spans="2:2" ht="13" x14ac:dyDescent="0.15">
-      <c r="B105" s="33"/>
+      <c r="B105" s="32"/>
     </row>
     <row r="106" spans="2:2" ht="13" x14ac:dyDescent="0.15">
-      <c r="B106" s="33"/>
+      <c r="B106" s="32"/>
     </row>
     <row r="107" spans="2:2" ht="13" x14ac:dyDescent="0.15">
-      <c r="B107" s="33"/>
+      <c r="B107" s="32"/>
     </row>
     <row r="108" spans="2:2" ht="13" x14ac:dyDescent="0.15">
-      <c r="B108" s="33"/>
+      <c r="B108" s="32"/>
     </row>
     <row r="109" spans="2:2" ht="13" x14ac:dyDescent="0.15">
-      <c r="B109" s="33"/>
+      <c r="B109" s="32"/>
     </row>
     <row r="110" spans="2:2" ht="13" x14ac:dyDescent="0.15">
-      <c r="B110" s="33"/>
+      <c r="B110" s="32"/>
     </row>
     <row r="111" spans="2:2" ht="13" x14ac:dyDescent="0.15">
-      <c r="B111" s="33"/>
+      <c r="B111" s="32"/>
     </row>
     <row r="112" spans="2:2" ht="13" x14ac:dyDescent="0.15">
-      <c r="B112" s="34"/>
+      <c r="B112" s="33"/>
     </row>
     <row r="113" spans="2:2" ht="13" x14ac:dyDescent="0.15">
-      <c r="B113" s="33"/>
+      <c r="B113" s="32"/>
     </row>
     <row r="114" spans="2:2" ht="13" x14ac:dyDescent="0.15">
-      <c r="B114" s="33"/>
+      <c r="B114" s="32"/>
     </row>
     <row r="115" spans="2:2" ht="13" x14ac:dyDescent="0.15">
-      <c r="B115" s="33"/>
+      <c r="B115" s="32"/>
     </row>
     <row r="116" spans="2:2" ht="13" x14ac:dyDescent="0.15">
-      <c r="B116" s="33"/>
+      <c r="B116" s="32"/>
     </row>
     <row r="117" spans="2:2" ht="13" x14ac:dyDescent="0.15">
-      <c r="B117" s="33"/>
+      <c r="B117" s="32"/>
     </row>
     <row r="118" spans="2:2" ht="13" x14ac:dyDescent="0.15">
-      <c r="B118" s="33"/>
+      <c r="B118" s="32"/>
     </row>
     <row r="119" spans="2:2" ht="13" x14ac:dyDescent="0.15">
-      <c r="B119" s="33"/>
+      <c r="B119" s="32"/>
     </row>
     <row r="120" spans="2:2" ht="13" x14ac:dyDescent="0.15">
-      <c r="B120" s="33"/>
+      <c r="B120" s="32"/>
     </row>
     <row r="121" spans="2:2" ht="13" x14ac:dyDescent="0.15">
-      <c r="B121" s="33"/>
+      <c r="B121" s="32"/>
     </row>
     <row r="122" spans="2:2" ht="13" x14ac:dyDescent="0.15">
-      <c r="B122" s="33"/>
+      <c r="B122" s="32"/>
     </row>
     <row r="123" spans="2:2" ht="13" x14ac:dyDescent="0.15">
-      <c r="B123" s="33"/>
+      <c r="B123" s="32"/>
     </row>
     <row r="124" spans="2:2" ht="13" x14ac:dyDescent="0.15">
-      <c r="B124" s="33"/>
+      <c r="B124" s="32"/>
     </row>
     <row r="125" spans="2:2" ht="13" x14ac:dyDescent="0.15">
-      <c r="B125" s="33"/>
+      <c r="B125" s="32"/>
     </row>
     <row r="126" spans="2:2" ht="13" x14ac:dyDescent="0.15">
-      <c r="B126" s="33"/>
+      <c r="B126" s="32"/>
     </row>
     <row r="127" spans="2:2" ht="13" x14ac:dyDescent="0.15">
-      <c r="B127" s="33"/>
+      <c r="B127" s="32"/>
     </row>
     <row r="128" spans="2:2" ht="13" x14ac:dyDescent="0.15">
-      <c r="B128" s="33"/>
+      <c r="B128" s="32"/>
     </row>
     <row r="129" spans="2:2" ht="13" x14ac:dyDescent="0.15">
-      <c r="B129" s="33"/>
+      <c r="B129" s="32"/>
     </row>
     <row r="130" spans="2:2" ht="13" x14ac:dyDescent="0.15">
-      <c r="B130" s="33"/>
+      <c r="B130" s="32"/>
     </row>
     <row r="131" spans="2:2" ht="13" x14ac:dyDescent="0.15">
-      <c r="B131" s="33"/>
+      <c r="B131" s="32"/>
     </row>
     <row r="132" spans="2:2" ht="13" x14ac:dyDescent="0.15">
-      <c r="B132" s="33"/>
+      <c r="B132" s="32"/>
     </row>
     <row r="133" spans="2:2" ht="13" x14ac:dyDescent="0.15">
-      <c r="B133" s="33"/>
+      <c r="B133" s="32"/>
     </row>
     <row r="134" spans="2:2" ht="13" x14ac:dyDescent="0.15">
-      <c r="B134" s="33"/>
+      <c r="B134" s="32"/>
     </row>
     <row r="135" spans="2:2" ht="13" x14ac:dyDescent="0.15">
-      <c r="B135" s="33"/>
+      <c r="B135" s="32"/>
     </row>
     <row r="136" spans="2:2" ht="13" x14ac:dyDescent="0.15">
-      <c r="B136" s="33"/>
+      <c r="B136" s="32"/>
     </row>
     <row r="137" spans="2:2" ht="13" x14ac:dyDescent="0.15">
-      <c r="B137" s="33"/>
+      <c r="B137" s="32"/>
     </row>
     <row r="138" spans="2:2" ht="13" x14ac:dyDescent="0.15">
-      <c r="B138" s="33"/>
+      <c r="B138" s="32"/>
     </row>
     <row r="139" spans="2:2" ht="13" x14ac:dyDescent="0.15">
-      <c r="B139" s="33"/>
+      <c r="B139" s="32"/>
     </row>
     <row r="140" spans="2:2" ht="13" x14ac:dyDescent="0.15">
-      <c r="B140" s="34"/>
+      <c r="B140" s="33"/>
     </row>
     <row r="141" spans="2:2" ht="13" x14ac:dyDescent="0.15">
-      <c r="B141" s="33"/>
+      <c r="B141" s="32"/>
     </row>
     <row r="142" spans="2:2" ht="13" x14ac:dyDescent="0.15">
-      <c r="B142" s="33"/>
+      <c r="B142" s="32"/>
     </row>
     <row r="143" spans="2:2" ht="13" x14ac:dyDescent="0.15">
-      <c r="B143" s="33"/>
+      <c r="B143" s="32"/>
     </row>
     <row r="144" spans="2:2" ht="13" x14ac:dyDescent="0.15">
-      <c r="B144" s="33"/>
+      <c r="B144" s="32"/>
     </row>
     <row r="145" spans="2:2" ht="13" x14ac:dyDescent="0.15">
-      <c r="B145" s="33"/>
+      <c r="B145" s="32"/>
     </row>
     <row r="146" spans="2:2" ht="13" x14ac:dyDescent="0.15">
-      <c r="B146" s="33"/>
+      <c r="B146" s="32"/>
     </row>
     <row r="147" spans="2:2" ht="13" x14ac:dyDescent="0.15">
-      <c r="B147" s="33"/>
+      <c r="B147" s="32"/>
     </row>
     <row r="148" spans="2:2" ht="13" x14ac:dyDescent="0.15">
-      <c r="B148" s="33"/>
+      <c r="B148" s="32"/>
     </row>
     <row r="149" spans="2:2" ht="13" x14ac:dyDescent="0.15">
-      <c r="B149" s="33"/>
+      <c r="B149" s="32"/>
     </row>
     <row r="150" spans="2:2" ht="13" x14ac:dyDescent="0.15">
-      <c r="B150" s="33"/>
+      <c r="B150" s="32"/>
     </row>
     <row r="151" spans="2:2" ht="13" x14ac:dyDescent="0.15">
-      <c r="B151" s="33"/>
+      <c r="B151" s="32"/>
     </row>
     <row r="152" spans="2:2" ht="13" x14ac:dyDescent="0.15">
-      <c r="B152" s="33"/>
+      <c r="B152" s="32"/>
     </row>
     <row r="153" spans="2:2" ht="13" x14ac:dyDescent="0.15">
-      <c r="B153" s="34"/>
+      <c r="B153" s="33"/>
     </row>
     <row r="154" spans="2:2" ht="13" x14ac:dyDescent="0.15">
-      <c r="B154" s="33"/>
+      <c r="B154" s="32"/>
     </row>
     <row r="155" spans="2:2" ht="13" x14ac:dyDescent="0.15">
-      <c r="B155" s="33"/>
+      <c r="B155" s="32"/>
     </row>
     <row r="156" spans="2:2" ht="13" x14ac:dyDescent="0.15">
-      <c r="B156" s="33"/>
+      <c r="B156" s="32"/>
     </row>
   </sheetData>
   <autoFilter ref="A1:D78" xr:uid="{00000000-0009-0000-0000-000006000000}">

</xml_diff>